<commit_message>
Reset Zone and UI
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 ChecklistFinal.xlsx
+++ b/AGA206 Assessment 2 ChecklistFinal.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\UNI Assessments\Trimester 2\Games Dev AGA206\Roll-A-Ball\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pissa2\WorkSpaceJune23\AGA206\Roll-A-Ball\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F3A194-9F7A-4077-A327-6A9AF83FE9E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5535" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="5535" windowWidth="25440" windowHeight="15270"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -155,7 +154,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -391,7 +390,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -403,7 +402,7 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -502,7 +501,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$13" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$13" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -530,11 +529,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$14" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$14" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$15" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$15" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -564,15 +563,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>30480</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -631,15 +630,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>175260</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -698,15 +697,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>175260</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -765,15 +764,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>175260</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -832,13 +831,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>160020</xdr:rowOff>
+          <xdr:rowOff>161925</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -899,13 +898,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>19</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -966,13 +965,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1033,15 +1032,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>19</xdr:row>
-          <xdr:rowOff>121920</xdr:rowOff>
+          <xdr:rowOff>123825</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>30480</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1100,15 +1099,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>20</xdr:row>
-          <xdr:rowOff>121920</xdr:rowOff>
+          <xdr:rowOff>123825</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>30480</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1167,13 +1166,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>23</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1234,13 +1233,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>24</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1301,15 +1300,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>23</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>25</xdr:row>
-          <xdr:rowOff>22860</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1368,13 +1367,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>24</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>26</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1435,13 +1434,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>25</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>27</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1502,13 +1501,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>26</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>28</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1569,13 +1568,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>27</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>29</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1636,13 +1635,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>28</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>30</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1703,13 +1702,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>29</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>31</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1770,13 +1769,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>30</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>32</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1837,13 +1836,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>31</xdr:row>
-          <xdr:rowOff>144780</xdr:rowOff>
+          <xdr:rowOff>142875</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>33</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1904,15 +1903,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>32</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>34</xdr:row>
-          <xdr:rowOff>45720</xdr:rowOff>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1971,13 +1970,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>33</xdr:row>
-          <xdr:rowOff>144780</xdr:rowOff>
+          <xdr:rowOff>142875</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>35</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -2038,13 +2037,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>34</xdr:row>
-          <xdr:rowOff>144780</xdr:rowOff>
+          <xdr:rowOff>142875</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>36</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -2105,13 +2104,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>35</xdr:row>
-          <xdr:rowOff>144780</xdr:rowOff>
+          <xdr:rowOff>142875</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>37</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -2172,13 +2171,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>36</xdr:row>
-          <xdr:rowOff>144780</xdr:rowOff>
+          <xdr:rowOff>142875</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>38</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -2499,31 +2498,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.90625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="6.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.6328125" style="14" customWidth="1"/>
-    <col min="4" max="4" width="7.453125" style="20" customWidth="1"/>
-    <col min="5" max="5" width="7.6328125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.08984375" style="9" customWidth="1"/>
-    <col min="7" max="7" width="50.26953125" style="14" customWidth="1"/>
-    <col min="8" max="8" width="9.90625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="1.875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="6.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="7.5" style="20" customWidth="1"/>
+    <col min="5" max="5" width="7.625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="50.25" style="14" customWidth="1"/>
+    <col min="8" max="8" width="9.875" style="2" customWidth="1"/>
     <col min="9" max="9" width="10" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="5.08984375" style="2" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="5.125" style="2" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="6" style="2" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="9.08984375" style="2" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="9.125" style="2" hidden="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C2" s="23" t="s">
         <v>34</v>
       </c>
@@ -2531,14 +2530,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="29" t="s">
         <v>37</v>
       </c>
       <c r="E4" s="27"/>
@@ -2547,11 +2546,11 @@
       <c r="H4" s="22"/>
       <c r="I4" s="22"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="26" t="s">
         <v>36</v>
       </c>
       <c r="E5" s="27"/>
@@ -2560,20 +2559,20 @@
       <c r="H5" s="22"/>
       <c r="I5" s="22"/>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C7" s="7" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="8">
         <f>COUNTIFS(J12:J15,TRUE)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C8" s="7" t="s">
         <v>31</v>
       </c>
@@ -2582,7 +2581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C9" s="7" t="s">
         <v>33</v>
       </c>
@@ -2591,7 +2590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
@@ -2612,7 +2611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6">
         <v>1</v>
       </c>
@@ -2632,7 +2631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6">
         <v>2</v>
       </c>
@@ -2645,14 +2644,14 @@
       <c r="E13" s="7"/>
       <c r="F13" s="6" t="str">
         <f>IF(J13,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G13" s="17"/>
       <c r="J13" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6">
         <v>3</v>
       </c>
@@ -2665,14 +2664,14 @@
       <c r="E14" s="7"/>
       <c r="F14" s="6" t="str">
         <f>IF(J14,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G14" s="17"/>
       <c r="J14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6">
         <v>4</v>
       </c>
@@ -2685,17 +2684,17 @@
       <c r="E15" s="7"/>
       <c r="F15" s="6" t="str">
         <f>IF(J15,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G15" s="17"/>
       <c r="J15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="9"/>
     </row>
-    <row r="17" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="10" t="s">
         <v>2</v>
       </c>
@@ -2713,7 +2712,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="6">
         <v>5</v>
       </c>
@@ -2737,7 +2736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="6">
         <v>6</v>
       </c>
@@ -2761,7 +2760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="6">
         <v>7</v>
       </c>
@@ -2785,7 +2784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="6">
         <v>8</v>
       </c>
@@ -2809,7 +2808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="6">
         <v>9</v>
       </c>
@@ -2833,7 +2832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="6">
         <v>10</v>
       </c>
@@ -2857,7 +2856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="6">
         <v>11</v>
       </c>
@@ -2881,7 +2880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="6">
         <v>12</v>
       </c>
@@ -2905,7 +2904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="6">
         <v>13</v>
       </c>
@@ -2929,7 +2928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27" s="6">
         <v>14</v>
       </c>
@@ -2953,7 +2952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28" s="6">
         <v>15</v>
       </c>
@@ -2977,7 +2976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" s="6">
         <v>16</v>
       </c>
@@ -3001,7 +3000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30" s="6">
         <v>17</v>
       </c>
@@ -3025,7 +3024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B31" s="6">
         <v>18</v>
       </c>
@@ -3049,7 +3048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="6">
         <v>19</v>
       </c>
@@ -3073,7 +3072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" s="6">
         <v>20</v>
       </c>
@@ -3097,7 +3096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" s="6">
         <v>21</v>
       </c>
@@ -3121,7 +3120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="6">
         <v>22</v>
       </c>
@@ -3145,7 +3144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="6">
         <v>23</v>
       </c>
@@ -3169,7 +3168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="6">
         <v>24</v>
       </c>
@@ -3193,7 +3192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B38" s="6">
         <v>25</v>
       </c>
@@ -3217,7 +3216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="K39" s="2">
         <f>SUM(K18:K38)</f>
         <v>0</v>
@@ -3244,7 +3243,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" xr:uid="{80E76939-EA24-4ADF-9C66-B313DF3F6F70}"/>
+    <hyperlink ref="D5" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="portrait" r:id="rId2"/>
@@ -3260,15 +3259,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>11</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>12</xdr:row>
-                    <xdr:rowOff>30480</xdr:rowOff>
+                    <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3282,15 +3281,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>11</xdr:row>
-                    <xdr:rowOff>175260</xdr:rowOff>
+                    <xdr:rowOff>171450</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>13</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3304,15 +3303,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>12</xdr:row>
-                    <xdr:rowOff>175260</xdr:rowOff>
+                    <xdr:rowOff>171450</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>14</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3326,15 +3325,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>13</xdr:row>
-                    <xdr:rowOff>175260</xdr:rowOff>
+                    <xdr:rowOff>171450</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3348,13 +3347,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>16</xdr:row>
-                    <xdr:rowOff>160020</xdr:rowOff>
+                    <xdr:rowOff>161925</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>18</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3370,13 +3369,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>17</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>19</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3392,13 +3391,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>18</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>20</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3414,15 +3413,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>19</xdr:row>
-                    <xdr:rowOff>121920</xdr:rowOff>
+                    <xdr:rowOff>123825</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>21</xdr:row>
-                    <xdr:rowOff>30480</xdr:rowOff>
+                    <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3436,15 +3435,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>20</xdr:row>
-                    <xdr:rowOff>121920</xdr:rowOff>
+                    <xdr:rowOff>123825</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>22</xdr:row>
-                    <xdr:rowOff>30480</xdr:rowOff>
+                    <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3458,13 +3457,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>21</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>23</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3480,13 +3479,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>22</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>24</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3502,15 +3501,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>23</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>25</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3524,13 +3523,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>24</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>26</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3546,13 +3545,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>25</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>27</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3568,13 +3567,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>26</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>28</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3590,13 +3589,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>27</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>29</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3612,13 +3611,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>28</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>30</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3634,13 +3633,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>29</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>31</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3656,13 +3655,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>30</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>32</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3678,13 +3677,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>31</xdr:row>
-                    <xdr:rowOff>144780</xdr:rowOff>
+                    <xdr:rowOff>142875</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>33</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3700,15 +3699,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>32</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>34</xdr:row>
-                    <xdr:rowOff>45720</xdr:rowOff>
+                    <xdr:rowOff>47625</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3722,13 +3721,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>33</xdr:row>
-                    <xdr:rowOff>144780</xdr:rowOff>
+                    <xdr:rowOff>142875</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>35</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3744,13 +3743,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>34</xdr:row>
-                    <xdr:rowOff>144780</xdr:rowOff>
+                    <xdr:rowOff>142875</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>36</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3766,13 +3765,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>35</xdr:row>
-                    <xdr:rowOff>144780</xdr:rowOff>
+                    <xdr:rowOff>142875</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>37</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3788,13 +3787,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>36</xdr:row>
-                    <xdr:rowOff>144780</xdr:rowOff>
+                    <xdr:rowOff>142875</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>38</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>

</xml_diff>

<commit_message>
Cameral following and rotating
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 ChecklistFinal.xlsx
+++ b/AGA206 Assessment 2 ChecklistFinal.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pissa2\WorkSpaceJune23\AGA206\Roll-A-Ball\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\UNI Assessments\Trimester 2\Games Dev AGA206\Roll-A-Ball\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF89D4B-5355-4F7C-8365-DD92A48B2FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5535" windowWidth="25440" windowHeight="15270"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -154,8 +155,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -207,12 +208,6 @@
       <color theme="10"/>
       <name val="Verdana"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -328,7 +323,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -396,6 +391,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -411,12 +409,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -485,11 +477,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$26" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$26" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$27" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$27" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
@@ -575,15 +567,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>30480</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -642,15 +634,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>175260</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>7620</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -709,15 +701,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>175260</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>7620</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -776,15 +768,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>175260</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>7620</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -843,13 +835,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
+          <xdr:rowOff>160020</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -910,13 +902,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>19</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -977,13 +969,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1044,15 +1036,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>19</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:rowOff>121920</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>30480</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1111,15 +1103,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>20</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:rowOff>121920</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>30480</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1178,13 +1170,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>23</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1245,13 +1237,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>24</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1312,15 +1304,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>23</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>25</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1379,13 +1371,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>24</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>26</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1446,13 +1438,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>25</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>27</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1513,13 +1505,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>26</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>28</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1580,13 +1572,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>27</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>29</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1647,13 +1639,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>28</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>30</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1714,13 +1706,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>29</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>31</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1781,13 +1773,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>30</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>32</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1848,13 +1840,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>31</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>33</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1915,15 +1907,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>32</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>34</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1982,13 +1974,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>33</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>35</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -2049,13 +2041,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>34</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>36</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -2116,13 +2108,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>35</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>37</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -2183,13 +2175,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>36</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>38</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -2510,31 +2502,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="6.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="7.5" style="20" customWidth="1"/>
-    <col min="5" max="5" width="7.625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="50.25" style="14" customWidth="1"/>
-    <col min="8" max="8" width="9.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="1.90625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="6.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.6328125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" style="20" customWidth="1"/>
+    <col min="5" max="5" width="7.6328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.08984375" style="9" customWidth="1"/>
+    <col min="7" max="7" width="50.26953125" style="14" customWidth="1"/>
+    <col min="8" max="8" width="9.90625" style="2" customWidth="1"/>
     <col min="9" max="9" width="10" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="5.125" style="2" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="5.08984375" style="2" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="6" style="2" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="9.125" style="2" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="9.08984375" style="2" hidden="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C2" s="23" t="s">
         <v>34</v>
       </c>
@@ -2542,40 +2534,40 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="29"/>
       <c r="H4" s="22"/>
       <c r="I4" s="22"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="29"/>
       <c r="H5" s="22"/>
       <c r="I5" s="22"/>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C7" s="7" t="s">
         <v>30</v>
       </c>
@@ -2584,25 +2576,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C8" s="7" t="s">
         <v>31</v>
       </c>
       <c r="D8" s="8">
         <f>COUNTIFS(J18:J38,TRUE)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C9" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D9" s="8">
         <f>K39</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
@@ -2623,7 +2615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="6">
         <v>1</v>
       </c>
@@ -2643,7 +2635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="6">
         <v>2</v>
       </c>
@@ -2663,7 +2655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="6">
         <v>3</v>
       </c>
@@ -2683,7 +2675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="6">
         <v>4</v>
       </c>
@@ -2703,10 +2695,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="9"/>
     </row>
-    <row r="17" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="10" t="s">
         <v>2</v>
       </c>
@@ -2724,11 +2716,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" s="6">
         <v>5</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="25" t="s">
         <v>11</v>
       </c>
       <c r="D18" s="19">
@@ -2748,7 +2740,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" s="6">
         <v>6</v>
       </c>
@@ -2772,7 +2764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" s="6">
         <v>7</v>
       </c>
@@ -2796,7 +2788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="6">
         <v>8</v>
       </c>
@@ -2820,7 +2812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" s="6">
         <v>9</v>
       </c>
@@ -2844,7 +2836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" s="6">
         <v>10</v>
       </c>
@@ -2868,7 +2860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" s="6">
         <v>11</v>
       </c>
@@ -2892,7 +2884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" s="6">
         <v>12</v>
       </c>
@@ -2916,7 +2908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" s="6">
         <v>13</v>
       </c>
@@ -2929,22 +2921,22 @@
       <c r="E26" s="7"/>
       <c r="F26" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G26" s="17"/>
       <c r="J26" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B27" s="6">
         <v>14</v>
       </c>
-      <c r="C27" s="30" t="s">
+      <c r="C27" s="26" t="s">
         <v>20</v>
       </c>
       <c r="D27" s="19">
@@ -2953,18 +2945,18 @@
       <c r="E27" s="7"/>
       <c r="F27" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G27" s="17"/>
       <c r="J27" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" s="6">
         <v>15</v>
       </c>
@@ -2988,7 +2980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29" s="6">
         <v>16</v>
       </c>
@@ -3012,7 +3004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B30" s="6">
         <v>17</v>
       </c>
@@ -3036,7 +3028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B31" s="6">
         <v>18</v>
       </c>
@@ -3060,7 +3052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B32" s="6">
         <v>19</v>
       </c>
@@ -3084,11 +3076,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B33" s="6">
         <v>20</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="25" t="s">
         <v>26</v>
       </c>
       <c r="D33" s="19">
@@ -3108,11 +3100,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B34" s="6">
         <v>21</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="25" t="s">
         <v>27</v>
       </c>
       <c r="D34" s="19">
@@ -3132,7 +3124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B35" s="6">
         <v>22</v>
       </c>
@@ -3156,7 +3148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B36" s="6">
         <v>23</v>
       </c>
@@ -3180,7 +3172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B37" s="6">
         <v>24</v>
       </c>
@@ -3204,7 +3196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B38" s="6">
         <v>25</v>
       </c>
@@ -3228,10 +3220,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
       <c r="K39" s="2">
         <f>SUM(K18:K38)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -3255,7 +3247,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="portrait" r:id="rId2"/>
@@ -3271,15 +3263,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>11</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>12</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>30480</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3293,15 +3285,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>11</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>175260</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>13</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>7620</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3315,15 +3307,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>12</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>175260</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>14</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>7620</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3337,15 +3329,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>13</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>175260</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>7620</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3359,13 +3351,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>16</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
+                    <xdr:rowOff>160020</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>18</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3381,13 +3373,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>17</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>19</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3403,13 +3395,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>18</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>20</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3425,15 +3417,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>19</xdr:row>
-                    <xdr:rowOff>123825</xdr:rowOff>
+                    <xdr:rowOff>121920</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>21</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>30480</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3447,15 +3439,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>20</xdr:row>
-                    <xdr:rowOff>123825</xdr:rowOff>
+                    <xdr:rowOff>121920</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>22</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>30480</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3469,13 +3461,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>21</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>23</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3491,13 +3483,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>22</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>24</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3513,15 +3505,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>23</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>25</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3535,13 +3527,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>24</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>26</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3557,13 +3549,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>25</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>27</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3579,13 +3571,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>26</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>28</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3601,13 +3593,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>27</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>29</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3623,13 +3615,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>28</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>30</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3645,13 +3637,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>29</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>31</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3667,13 +3659,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>30</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>32</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3689,13 +3681,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>31</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:rowOff>144780</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>33</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3711,15 +3703,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>32</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>34</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
+                    <xdr:rowOff>45720</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3733,13 +3725,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>33</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:rowOff>144780</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>35</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3755,13 +3747,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>34</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:rowOff>144780</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>36</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3777,13 +3769,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>35</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:rowOff>144780</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>37</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3799,13 +3791,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>36</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:rowOff>144780</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>38</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>

</xml_diff>

<commit_message>
BowlingMap Created Neon Lights
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 ChecklistFinal.xlsx
+++ b/AGA206 Assessment 2 ChecklistFinal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\UNI Assessments\Trimester 2\Games Dev AGA206\Roll-A-Ball\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3C8F75-C429-40EB-916E-50ECA9385A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42422F78-E487-4F16-8B33-97F1662EFB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -210,7 +210,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -226,6 +226,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -323,7 +329,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -391,9 +397,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -409,6 +412,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -493,11 +516,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$30" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$30" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$31" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$31" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2506,7 +2529,7 @@
   <dimension ref="B2:L39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -2541,12 +2564,12 @@
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="29"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="28"/>
       <c r="H4" s="22"/>
       <c r="I4" s="22"/>
     </row>
@@ -2554,12 +2577,12 @@
       <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="29"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="28"/>
       <c r="H5" s="22"/>
       <c r="I5" s="22"/>
     </row>
@@ -2582,7 +2605,7 @@
       </c>
       <c r="D8" s="8">
         <f>COUNTIFS(J18:J38,TRUE)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
@@ -2591,7 +2614,7 @@
       </c>
       <c r="D9" s="8">
         <f>K39</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2741,21 +2764,21 @@
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B19" s="6">
+      <c r="B19" s="30">
         <v>6</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="32">
         <v>2</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="6" t="str">
+      <c r="E19" s="33"/>
+      <c r="F19" s="30" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G19" s="17"/>
+      <c r="G19" s="34"/>
       <c r="J19" s="5" t="b">
         <v>0</v>
       </c>
@@ -2789,21 +2812,21 @@
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B21" s="6">
+      <c r="B21" s="30">
         <v>8</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="32">
         <v>2</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="6" t="str">
+      <c r="E21" s="33"/>
+      <c r="F21" s="30" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G21" s="17"/>
+      <c r="G21" s="34"/>
       <c r="J21" s="5" t="b">
         <v>0</v>
       </c>
@@ -2837,21 +2860,21 @@
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B23" s="6">
+      <c r="B23" s="30">
         <v>10</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="19">
+      <c r="D23" s="32">
         <v>1</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="6" t="str">
+      <c r="E23" s="33"/>
+      <c r="F23" s="30" t="str">
         <f t="shared" si="0"/>
         <v>Done</v>
       </c>
-      <c r="G23" s="17"/>
+      <c r="G23" s="34"/>
       <c r="J23" s="5" t="b">
         <v>1</v>
       </c>
@@ -2885,21 +2908,21 @@
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B25" s="6">
+      <c r="B25" s="30">
         <v>12</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="19">
+      <c r="D25" s="32">
         <v>1</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="6" t="str">
+      <c r="E25" s="33"/>
+      <c r="F25" s="30" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G25" s="17"/>
+      <c r="G25" s="34"/>
       <c r="J25" s="5" t="b">
         <v>0</v>
       </c>
@@ -2933,21 +2956,21 @@
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B27" s="6">
+      <c r="B27" s="30">
         <v>14</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="19">
+      <c r="D27" s="32">
         <v>1</v>
       </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="6" t="str">
+      <c r="E27" s="33"/>
+      <c r="F27" s="30" t="str">
         <f t="shared" si="0"/>
         <v>Done</v>
       </c>
-      <c r="G27" s="17"/>
+      <c r="G27" s="34"/>
       <c r="J27" s="5" t="b">
         <v>1</v>
       </c>
@@ -2981,21 +3004,21 @@
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B29" s="6">
+      <c r="B29" s="30">
         <v>16</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="19">
+      <c r="D29" s="32">
         <v>1</v>
       </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="6" t="str">
+      <c r="E29" s="33"/>
+      <c r="F29" s="30" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G29" s="17"/>
+      <c r="G29" s="34"/>
       <c r="J29" s="5" t="b">
         <v>0</v>
       </c>
@@ -3017,39 +3040,39 @@
       <c r="E30" s="7"/>
       <c r="F30" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G30" s="17"/>
       <c r="J30" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B31" s="6">
+      <c r="B31" s="30">
         <v>18</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="19">
+      <c r="D31" s="32">
         <v>1</v>
       </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="6" t="str">
+      <c r="E31" s="33"/>
+      <c r="F31" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
-      </c>
-      <c r="G31" s="17"/>
+        <v>Done</v>
+      </c>
+      <c r="G31" s="34"/>
       <c r="J31" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.3">
@@ -3077,21 +3100,21 @@
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B33" s="6">
+      <c r="B33" s="30">
         <v>20</v>
       </c>
-      <c r="C33" s="25" t="s">
+      <c r="C33" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="D33" s="19">
+      <c r="D33" s="32">
         <v>1</v>
       </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="6" t="str">
+      <c r="E33" s="33"/>
+      <c r="F33" s="30" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G33" s="17"/>
+      <c r="G33" s="34"/>
       <c r="J33" s="5" t="b">
         <v>0</v>
       </c>
@@ -3125,21 +3148,21 @@
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B35" s="6">
+      <c r="B35" s="30">
         <v>22</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="19">
+      <c r="D35" s="32">
         <v>2</v>
       </c>
-      <c r="E35" s="7"/>
-      <c r="F35" s="6" t="str">
+      <c r="E35" s="33"/>
+      <c r="F35" s="30" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G35" s="17"/>
+      <c r="G35" s="34"/>
       <c r="J35" s="5" t="b">
         <v>0</v>
       </c>
@@ -3173,21 +3196,21 @@
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B37" s="6">
+      <c r="B37" s="30">
         <v>24</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="19">
+      <c r="D37" s="32">
         <v>1</v>
       </c>
-      <c r="E37" s="7"/>
-      <c r="F37" s="6" t="str">
+      <c r="E37" s="33"/>
+      <c r="F37" s="30" t="str">
         <f t="shared" si="2"/>
         <v>To Be Done</v>
       </c>
-      <c r="G37" s="17"/>
+      <c r="G37" s="34"/>
       <c r="J37" s="5" t="b">
         <v>0</v>
       </c>
@@ -3223,7 +3246,7 @@
     <row r="39" spans="2:11" x14ac:dyDescent="0.3">
       <c r="K39" s="2">
         <f>SUM(K18:K38)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TryingTo Animate Death Beam
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 ChecklistFinal.xlsx
+++ b/AGA206 Assessment 2 ChecklistFinal.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\UNI Assessments\Trimester 2\Games Dev AGA206\Roll-A-Ball\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pissa2\WorkSpaceJune23\AGA206\Roll-A-Ball\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42422F78-E487-4F16-8B33-97F1662EFB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16770"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>Status</t>
   </si>
@@ -151,11 +150,14 @@
   <si>
     <t>Patrick Issa</t>
   </si>
+  <si>
+    <t xml:space="preserve">Player Camera Controller </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -397,22 +399,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -432,6 +418,22 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -524,7 +526,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$32" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$32" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -540,7 +542,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$35" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$35" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
@@ -590,15 +592,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>30480</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -657,15 +659,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>175260</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -724,15 +726,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>175260</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -791,15 +793,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>175260</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -858,13 +860,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>160020</xdr:rowOff>
+          <xdr:rowOff>161925</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -925,13 +927,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>19</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -992,13 +994,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1059,15 +1061,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>19</xdr:row>
-          <xdr:rowOff>121920</xdr:rowOff>
+          <xdr:rowOff>123825</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>30480</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1126,15 +1128,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>20</xdr:row>
-          <xdr:rowOff>121920</xdr:rowOff>
+          <xdr:rowOff>123825</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>30480</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1193,13 +1195,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>23</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1260,13 +1262,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>24</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1327,15 +1329,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>23</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>25</xdr:row>
-          <xdr:rowOff>22860</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1394,13 +1396,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>24</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>26</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1461,13 +1463,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>25</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>27</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1528,13 +1530,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>26</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>28</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1595,13 +1597,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>27</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>29</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1662,13 +1664,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>28</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>30</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1729,13 +1731,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>29</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>31</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1796,13 +1798,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>30</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>32</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1863,13 +1865,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>31</xdr:row>
-          <xdr:rowOff>144780</xdr:rowOff>
+          <xdr:rowOff>142875</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>33</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1930,15 +1932,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>32</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>34</xdr:row>
-          <xdr:rowOff>45720</xdr:rowOff>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1997,13 +1999,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>33</xdr:row>
-          <xdr:rowOff>144780</xdr:rowOff>
+          <xdr:rowOff>142875</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>35</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -2064,13 +2066,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>34</xdr:row>
-          <xdr:rowOff>144780</xdr:rowOff>
+          <xdr:rowOff>142875</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>36</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -2131,13 +2133,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>35</xdr:row>
-          <xdr:rowOff>144780</xdr:rowOff>
+          <xdr:rowOff>142875</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>37</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -2198,13 +2200,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>198120</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>36</xdr:row>
-          <xdr:rowOff>144780</xdr:rowOff>
+          <xdr:rowOff>142875</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>38</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -2525,31 +2527,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.90625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="6.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.6328125" style="14" customWidth="1"/>
-    <col min="4" max="4" width="7.453125" style="20" customWidth="1"/>
-    <col min="5" max="5" width="7.6328125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.08984375" style="9" customWidth="1"/>
-    <col min="7" max="7" width="50.26953125" style="14" customWidth="1"/>
-    <col min="8" max="8" width="9.90625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="1.875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="6.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="7.5" style="20" customWidth="1"/>
+    <col min="5" max="5" width="7.625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="50.25" style="14" customWidth="1"/>
+    <col min="8" max="8" width="9.875" style="2" customWidth="1"/>
     <col min="9" max="9" width="10" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="5.08984375" style="2" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="5.125" style="2" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="6" style="2" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="9.08984375" style="2" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="9.125" style="2" hidden="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C2" s="23" t="s">
         <v>34</v>
       </c>
@@ -2557,40 +2559,40 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="28"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="35"/>
       <c r="H4" s="22"/>
       <c r="I4" s="22"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="28"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="35"/>
       <c r="H5" s="22"/>
       <c r="I5" s="22"/>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C7" s="7" t="s">
         <v>30</v>
       </c>
@@ -2599,25 +2601,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C8" s="7" t="s">
         <v>31</v>
       </c>
       <c r="D8" s="8">
         <f>COUNTIFS(J18:J38,TRUE)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C9" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D9" s="8">
         <f>K39</f>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
@@ -2638,7 +2640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6">
         <v>1</v>
       </c>
@@ -2658,7 +2660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6">
         <v>2</v>
       </c>
@@ -2678,7 +2680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6">
         <v>3</v>
       </c>
@@ -2698,7 +2700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6">
         <v>4</v>
       </c>
@@ -2718,10 +2720,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="9"/>
     </row>
-    <row r="17" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="10" t="s">
         <v>2</v>
       </c>
@@ -2739,7 +2741,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="6">
         <v>5</v>
       </c>
@@ -2763,22 +2765,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B19" s="30">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B19" s="26">
         <v>6</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="32">
+      <c r="D19" s="28">
         <v>2</v>
       </c>
-      <c r="E19" s="33"/>
-      <c r="F19" s="30" t="str">
+      <c r="E19" s="29"/>
+      <c r="F19" s="26" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G19" s="34"/>
+      <c r="G19" s="30"/>
       <c r="J19" s="5" t="b">
         <v>0</v>
       </c>
@@ -2787,7 +2789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="6">
         <v>7</v>
       </c>
@@ -2811,22 +2813,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B21" s="30">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B21" s="26">
         <v>8</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="32">
+      <c r="D21" s="28">
         <v>2</v>
       </c>
-      <c r="E21" s="33"/>
-      <c r="F21" s="30" t="str">
+      <c r="E21" s="29"/>
+      <c r="F21" s="26" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G21" s="34"/>
+      <c r="G21" s="30"/>
       <c r="J21" s="5" t="b">
         <v>0</v>
       </c>
@@ -2835,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="6">
         <v>9</v>
       </c>
@@ -2859,22 +2861,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B23" s="30">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B23" s="26">
         <v>10</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="32">
+      <c r="D23" s="28">
         <v>1</v>
       </c>
-      <c r="E23" s="33"/>
-      <c r="F23" s="30" t="str">
+      <c r="E23" s="29"/>
+      <c r="F23" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Done</v>
       </c>
-      <c r="G23" s="34"/>
+      <c r="G23" s="30"/>
       <c r="J23" s="5" t="b">
         <v>1</v>
       </c>
@@ -2883,7 +2885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="6">
         <v>11</v>
       </c>
@@ -2907,22 +2909,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B25" s="30">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B25" s="26">
         <v>12</v>
       </c>
-      <c r="C25" s="35" t="s">
+      <c r="C25" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="32">
+      <c r="D25" s="28">
         <v>1</v>
       </c>
-      <c r="E25" s="33"/>
-      <c r="F25" s="30" t="str">
+      <c r="E25" s="29"/>
+      <c r="F25" s="26" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G25" s="34"/>
+      <c r="G25" s="30"/>
       <c r="J25" s="5" t="b">
         <v>0</v>
       </c>
@@ -2931,7 +2933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="6">
         <v>13</v>
       </c>
@@ -2955,22 +2957,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B27" s="30">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B27" s="26">
         <v>14</v>
       </c>
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="32">
+      <c r="D27" s="28">
         <v>1</v>
       </c>
-      <c r="E27" s="33"/>
-      <c r="F27" s="30" t="str">
+      <c r="E27" s="29"/>
+      <c r="F27" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Done</v>
       </c>
-      <c r="G27" s="34"/>
+      <c r="G27" s="30"/>
       <c r="J27" s="5" t="b">
         <v>1</v>
       </c>
@@ -2979,7 +2981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28" s="6">
         <v>15</v>
       </c>
@@ -3003,22 +3005,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B29" s="30">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B29" s="26">
         <v>16</v>
       </c>
-      <c r="C29" s="31" t="s">
+      <c r="C29" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="32">
+      <c r="D29" s="28">
         <v>1</v>
       </c>
-      <c r="E29" s="33"/>
-      <c r="F29" s="30" t="str">
+      <c r="E29" s="29"/>
+      <c r="F29" s="26" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G29" s="34"/>
+      <c r="G29" s="30"/>
       <c r="J29" s="5" t="b">
         <v>0</v>
       </c>
@@ -3027,7 +3029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30" s="6">
         <v>17</v>
       </c>
@@ -3051,22 +3053,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B31" s="30">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B31" s="26">
         <v>18</v>
       </c>
-      <c r="C31" s="35" t="s">
+      <c r="C31" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="32">
+      <c r="D31" s="28">
         <v>1</v>
       </c>
-      <c r="E31" s="33"/>
-      <c r="F31" s="30" t="str">
+      <c r="E31" s="29"/>
+      <c r="F31" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Done</v>
       </c>
-      <c r="G31" s="34"/>
+      <c r="G31" s="30"/>
       <c r="J31" s="5" t="b">
         <v>1</v>
       </c>
@@ -3075,7 +3077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="6">
         <v>19</v>
       </c>
@@ -3088,33 +3090,33 @@
       <c r="E32" s="7"/>
       <c r="F32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G32" s="17"/>
       <c r="J32" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K32" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B33" s="30">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B33" s="26">
         <v>20</v>
       </c>
-      <c r="C33" s="35" t="s">
+      <c r="C33" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="D33" s="32">
+      <c r="D33" s="28">
         <v>1</v>
       </c>
-      <c r="E33" s="33"/>
-      <c r="F33" s="30" t="str">
+      <c r="E33" s="29"/>
+      <c r="F33" s="26" t="str">
         <f t="shared" si="0"/>
         <v>To Be Done</v>
       </c>
-      <c r="G33" s="34"/>
+      <c r="G33" s="30"/>
       <c r="J33" s="5" t="b">
         <v>0</v>
       </c>
@@ -3123,7 +3125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" s="6">
         <v>21</v>
       </c>
@@ -3147,31 +3149,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B35" s="30">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B35" s="26">
         <v>22</v>
       </c>
-      <c r="C35" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="D35" s="32">
+      <c r="C35" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="28">
         <v>2</v>
       </c>
-      <c r="E35" s="33"/>
-      <c r="F35" s="30" t="str">
+      <c r="E35" s="29"/>
+      <c r="F35" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
-      </c>
-      <c r="G35" s="34"/>
+        <v>Done</v>
+      </c>
+      <c r="G35" s="30"/>
       <c r="J35" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K35" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="6">
         <v>23</v>
       </c>
@@ -3195,22 +3197,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B37" s="30">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B37" s="26">
         <v>24</v>
       </c>
-      <c r="C37" s="31" t="s">
+      <c r="C37" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="32">
+      <c r="D37" s="28">
         <v>1</v>
       </c>
-      <c r="E37" s="33"/>
-      <c r="F37" s="30" t="str">
+      <c r="E37" s="29"/>
+      <c r="F37" s="26" t="str">
         <f t="shared" si="2"/>
         <v>To Be Done</v>
       </c>
-      <c r="G37" s="34"/>
+      <c r="G37" s="30"/>
       <c r="J37" s="5" t="b">
         <v>0</v>
       </c>
@@ -3219,7 +3221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B38" s="6">
         <v>25</v>
       </c>
@@ -3243,10 +3245,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="K39" s="2">
         <f>SUM(K18:K38)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -3270,7 +3272,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D5" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="portrait" r:id="rId2"/>
@@ -3286,15 +3288,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>11</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>12</xdr:row>
-                    <xdr:rowOff>30480</xdr:rowOff>
+                    <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3308,15 +3310,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>11</xdr:row>
-                    <xdr:rowOff>175260</xdr:rowOff>
+                    <xdr:rowOff>171450</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>13</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3330,15 +3332,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>12</xdr:row>
-                    <xdr:rowOff>175260</xdr:rowOff>
+                    <xdr:rowOff>171450</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>14</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3352,15 +3354,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>13</xdr:row>
-                    <xdr:rowOff>175260</xdr:rowOff>
+                    <xdr:rowOff>171450</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3374,13 +3376,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>16</xdr:row>
-                    <xdr:rowOff>160020</xdr:rowOff>
+                    <xdr:rowOff>161925</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>18</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3396,13 +3398,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>17</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>19</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3418,13 +3420,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>18</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>20</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3440,15 +3442,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>19</xdr:row>
-                    <xdr:rowOff>121920</xdr:rowOff>
+                    <xdr:rowOff>123825</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>21</xdr:row>
-                    <xdr:rowOff>30480</xdr:rowOff>
+                    <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3462,15 +3464,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>20</xdr:row>
-                    <xdr:rowOff>121920</xdr:rowOff>
+                    <xdr:rowOff>123825</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>22</xdr:row>
-                    <xdr:rowOff>30480</xdr:rowOff>
+                    <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3484,13 +3486,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>21</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>23</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3506,13 +3508,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>22</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>24</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3528,15 +3530,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>23</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>25</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3550,13 +3552,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>24</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>26</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3572,13 +3574,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>25</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>27</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3594,13 +3596,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>26</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>28</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3616,13 +3618,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>27</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>29</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3638,13 +3640,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>28</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>30</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3660,13 +3662,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>29</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>31</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3682,13 +3684,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>30</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>32</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3704,13 +3706,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>31</xdr:row>
-                    <xdr:rowOff>144780</xdr:rowOff>
+                    <xdr:rowOff>142875</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>33</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3726,15 +3728,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>32</xdr:row>
-                    <xdr:rowOff>137160</xdr:rowOff>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>34</xdr:row>
-                    <xdr:rowOff>45720</xdr:rowOff>
+                    <xdr:rowOff>47625</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3748,13 +3750,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>33</xdr:row>
-                    <xdr:rowOff>144780</xdr:rowOff>
+                    <xdr:rowOff>142875</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>35</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3770,13 +3772,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>34</xdr:row>
-                    <xdr:rowOff>144780</xdr:rowOff>
+                    <xdr:rowOff>142875</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>36</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3792,13 +3794,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>35</xdr:row>
-                    <xdr:rowOff>144780</xdr:rowOff>
+                    <xdr:rowOff>142875</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>37</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3814,13 +3816,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>198120</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>36</xdr:row>
-                    <xdr:rowOff>144780</xdr:rowOff>
+                    <xdr:rowOff>142875</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:colOff>476250</xdr:colOff>
                     <xdr:row>38</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>

</xml_diff>

<commit_message>
Free Cam and Pause Menu
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 ChecklistFinal.xlsx
+++ b/AGA206 Assessment 2 ChecklistFinal.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pissa2\WorkSpaceJune23\AGA206\Roll-A-Ball\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\UNI Assessments\Trimester 2\Games Dev AGA206\Roll-A-Ball\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E15A09D-66F2-4BE5-9BFB-A6348B9E7EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16770"/>
+    <workbookView xWindow="38280" yWindow="5535" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>Status</t>
   </si>
@@ -152,13 +153,16 @@
   </si>
   <si>
     <t>Wrong Way Barrier</t>
+  </si>
+  <si>
+    <t>Respawn Powerup Prefab</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -210,6 +214,13 @@
       <color theme="10"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -331,7 +342,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -435,6 +446,12 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -498,7 +515,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$25" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$25" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
@@ -526,7 +543,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$32" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$32" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -538,7 +555,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$34" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$34" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
@@ -546,7 +563,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$36" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$36" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
@@ -574,7 +591,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$20" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$20" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -592,15 +609,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>30480</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -659,15 +676,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>175260</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>7620</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -726,15 +743,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>175260</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>7620</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -793,15 +810,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>175260</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>7620</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -860,13 +877,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
+          <xdr:rowOff>160020</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -927,13 +944,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>19</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -994,13 +1011,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1061,15 +1078,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>19</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:rowOff>121920</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>30480</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1128,15 +1145,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>20</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:rowOff>121920</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>30480</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1195,13 +1212,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>23</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1262,13 +1279,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>24</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1329,15 +1346,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>23</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>25</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
+          <xdr:rowOff>22860</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1396,13 +1413,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>24</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>26</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1463,13 +1480,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>25</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>27</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1530,13 +1547,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>26</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>28</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1597,13 +1614,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>27</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>29</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1664,13 +1681,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>28</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>30</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1731,13 +1748,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>29</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>31</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1798,13 +1815,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>30</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>32</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1865,13 +1882,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>31</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>33</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -1932,15 +1949,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>32</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>34</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1999,13 +2016,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>33</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>35</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -2066,13 +2083,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>34</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>36</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -2133,13 +2150,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>35</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>37</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -2200,13 +2217,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:colOff>198120</xdr:colOff>
           <xdr:row>36</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:colOff>480060</xdr:colOff>
           <xdr:row>38</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -2527,31 +2544,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="6.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="7.5" style="20" customWidth="1"/>
-    <col min="5" max="5" width="7.625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="50.25" style="14" customWidth="1"/>
-    <col min="8" max="8" width="9.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="1.90625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="6.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.6328125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" style="20" customWidth="1"/>
+    <col min="5" max="5" width="7.6328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.08984375" style="9" customWidth="1"/>
+    <col min="7" max="7" width="50.26953125" style="14" customWidth="1"/>
+    <col min="8" max="8" width="9.90625" style="2" customWidth="1"/>
     <col min="9" max="9" width="10" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="5.125" style="2" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="5.08984375" style="2" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="6" style="2" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="9.125" style="2" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="9.08984375" style="2" hidden="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C2" s="23" t="s">
         <v>34</v>
       </c>
@@ -2559,10 +2576,10 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
@@ -2575,7 +2592,7 @@
       <c r="H4" s="22"/>
       <c r="I4" s="22"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
@@ -2588,11 +2605,11 @@
       <c r="H5" s="22"/>
       <c r="I5" s="22"/>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C7" s="7" t="s">
         <v>30</v>
       </c>
@@ -2601,25 +2618,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C8" s="7" t="s">
         <v>31</v>
       </c>
       <c r="D8" s="8">
         <f>COUNTIFS(J18:J38,TRUE)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C9" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D9" s="8">
         <f>K39</f>
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
@@ -2640,7 +2657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="6">
         <v>1</v>
       </c>
@@ -2660,7 +2677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="6">
         <v>2</v>
       </c>
@@ -2680,7 +2697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="6">
         <v>3</v>
       </c>
@@ -2700,7 +2717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="6">
         <v>4</v>
       </c>
@@ -2720,10 +2737,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="9"/>
     </row>
-    <row r="17" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="10" t="s">
         <v>2</v>
       </c>
@@ -2741,7 +2758,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" s="6">
         <v>5</v>
       </c>
@@ -2765,7 +2782,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" s="26">
         <v>6</v>
       </c>
@@ -2789,7 +2806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" s="6">
         <v>7</v>
       </c>
@@ -2802,18 +2819,18 @@
       <c r="E20" s="7"/>
       <c r="F20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G20" s="17"/>
       <c r="J20" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="26">
         <v>8</v>
       </c>
@@ -2837,7 +2854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" s="6">
         <v>9</v>
       </c>
@@ -2861,7 +2878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" s="26">
         <v>10</v>
       </c>
@@ -2885,11 +2902,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" s="6">
         <v>11</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="13" t="s">
         <v>17</v>
       </c>
       <c r="D24" s="19">
@@ -2909,7 +2926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" s="26">
         <v>12</v>
       </c>
@@ -2922,18 +2939,18 @@
       <c r="E25" s="29"/>
       <c r="F25" s="26" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G25" s="30"/>
       <c r="J25" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" s="6">
         <v>13</v>
       </c>
@@ -2957,7 +2974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B27" s="26">
         <v>14</v>
       </c>
@@ -2981,7 +2998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" s="6">
         <v>15</v>
       </c>
@@ -3005,7 +3022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29" s="26">
         <v>16</v>
       </c>
@@ -3029,7 +3046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B30" s="6">
         <v>17</v>
       </c>
@@ -3053,7 +3070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B31" s="26">
         <v>18</v>
       </c>
@@ -3077,11 +3094,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B32" s="6">
         <v>19</v>
       </c>
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="13" t="s">
         <v>25</v>
       </c>
       <c r="D32" s="19">
@@ -3090,22 +3107,22 @@
       <c r="E32" s="7"/>
       <c r="F32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>Done</v>
+        <v>To Be Done</v>
       </c>
       <c r="G32" s="17"/>
       <c r="J32" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K32" s="2">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B33" s="26">
         <v>20</v>
       </c>
-      <c r="C33" s="31" t="s">
+      <c r="C33" s="27" t="s">
         <v>26</v>
       </c>
       <c r="D33" s="28">
@@ -3125,7 +3142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B34" s="6">
         <v>21</v>
       </c>
@@ -3138,22 +3155,22 @@
       <c r="E34" s="7"/>
       <c r="F34" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G34" s="17"/>
       <c r="J34" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K34" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B35" s="26">
         <v>22</v>
       </c>
-      <c r="C35" s="27" t="s">
+      <c r="C35" s="38" t="s">
         <v>38</v>
       </c>
       <c r="D35" s="28">
@@ -3173,12 +3190,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B36" s="6">
         <v>23</v>
       </c>
-      <c r="C36" s="13" t="s">
-        <v>32</v>
+      <c r="C36" s="37" t="s">
+        <v>39</v>
       </c>
       <c r="D36" s="19">
         <v>2</v>
@@ -3186,18 +3203,18 @@
       <c r="E36" s="7"/>
       <c r="F36" s="6" t="str">
         <f t="shared" ref="F36:F38" si="2">IF(J36,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G36" s="17"/>
       <c r="J36" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K36" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B37" s="26">
         <v>24</v>
       </c>
@@ -3221,7 +3238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B38" s="6">
         <v>25</v>
       </c>
@@ -3245,10 +3262,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
       <c r="K39" s="2">
         <f>SUM(K18:K38)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -3272,7 +3289,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="portrait" r:id="rId2"/>
@@ -3288,15 +3305,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>11</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>12</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>30480</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3310,15 +3327,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>11</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>175260</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>13</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>7620</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3332,15 +3349,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>12</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>175260</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>14</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>7620</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3354,15 +3371,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>13</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
+                    <xdr:rowOff>175260</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>7620</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3376,13 +3393,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>16</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
+                    <xdr:rowOff>160020</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>18</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3398,13 +3415,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>17</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>19</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3420,13 +3437,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>18</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>20</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3442,15 +3459,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>19</xdr:row>
-                    <xdr:rowOff>123825</xdr:rowOff>
+                    <xdr:rowOff>121920</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>21</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>30480</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3464,15 +3481,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>20</xdr:row>
-                    <xdr:rowOff>123825</xdr:rowOff>
+                    <xdr:rowOff>121920</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>22</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>30480</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3486,13 +3503,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>21</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>23</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3508,13 +3525,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>22</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>24</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3530,15 +3547,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>23</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>25</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>22860</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3552,13 +3569,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>24</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>26</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3574,13 +3591,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>25</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>27</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3596,13 +3613,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>26</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>28</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3618,13 +3635,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>27</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>29</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3640,13 +3657,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>28</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>30</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3662,13 +3679,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>29</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>31</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3684,13 +3701,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>30</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>32</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3706,13 +3723,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>31</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:rowOff>144780</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>33</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3728,15 +3745,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>32</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>34</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
+                    <xdr:rowOff>45720</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3750,13 +3767,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>33</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:rowOff>144780</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>35</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3772,13 +3789,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>34</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:rowOff>144780</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>36</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3794,13 +3811,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>35</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:rowOff>144780</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>37</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -3816,13 +3833,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>36</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:rowOff>144780</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>476250</xdr:colOff>
+                    <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>38</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>

</xml_diff>